<commit_message>
Organisational practices model fit (not to use)
</commit_message>
<xml_diff>
--- a/Results/org_practices_modelfit.xlsx
+++ b/Results/org_practices_modelfit.xlsx
@@ -262,7 +262,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="3">
@@ -270,7 +270,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>9.87771468800886E-17</v>
+        <v>1.2710865025773388E-16</v>
       </c>
     </row>
     <row r="4">
@@ -278,7 +278,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.995515756285567E-12</v>
+        <v>3.894863261197482E-12</v>
       </c>
     </row>
     <row r="5">
@@ -302,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.995515756285567E-12</v>
+        <v>3.894863261197482E-12</v>
       </c>
     </row>
     <row r="8">
@@ -334,7 +334,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>18249.040911630796</v>
+        <v>17921.096717470624</v>
       </c>
     </row>
     <row r="12">
@@ -358,7 +358,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>18250.244515437127</v>
+        <v>17922.266501851664</v>
       </c>
     </row>
     <row r="15">
@@ -382,7 +382,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.9999340499901077</v>
+        <v>0.9999347301090005</v>
       </c>
     </row>
     <row r="18">
@@ -390,7 +390,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="19">
@@ -446,7 +446,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="26">
@@ -454,7 +454,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="27">
@@ -526,7 +526,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="36">
@@ -638,7 +638,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>4.1224459916953915E-9</v>
+        <v>4.9452456701650085E-9</v>
       </c>
     </row>
     <row r="50">
@@ -646,7 +646,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>5.048944585917745E-9</v>
+        <v>6.056664272306056E-9</v>
       </c>
     </row>
     <row r="51">
@@ -654,7 +654,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>5.048944585917745E-9</v>
+        <v>6.056664272306056E-9</v>
       </c>
     </row>
     <row r="52">
@@ -662,7 +662,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>4.1224459916953915E-9</v>
+        <v>4.9452456701650085E-9</v>
       </c>
     </row>
     <row r="53">
@@ -670,7 +670,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>5.048944585917745E-9</v>
+        <v>6.056664272306056E-9</v>
       </c>
     </row>
     <row r="54">
@@ -678,7 +678,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>5.048944585917745E-9</v>
+        <v>6.056664272306056E-9</v>
       </c>
     </row>
     <row r="55">
@@ -686,7 +686,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>7.1402859090750844E-9</v>
+        <v>8.565416756635797E-9</v>
       </c>
     </row>
     <row r="56">
@@ -726,7 +726,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="61">

</xml_diff>